<commit_message>
Automation of Balancesheet Test Cases added
</commit_message>
<xml_diff>
--- a/tests/artifact/script/DeliveryNote.xlsx
+++ b/tests/artifact/script/DeliveryNote.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -26528,13 +26528,13 @@
   <sheetPr/>
   <dimension ref="A1:O186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="$A20:$XFD20"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20" style="6" customWidth="1"/>
+    <col min="1" max="1" width="36.9" style="6" customWidth="1"/>
     <col min="2" max="2" width="32.3" style="7" customWidth="1"/>
     <col min="3" max="3" width="10.8333333333333" style="8" customWidth="1"/>
     <col min="4" max="4" width="30.8333333333333" style="9" customWidth="1"/>
@@ -31207,7 +31207,7 @@
   <sheetPr/>
   <dimension ref="A1:O211"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
@@ -35192,7 +35192,7 @@
   <sheetPr/>
   <dimension ref="A1:O208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>